<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@6bb7038cc7084867a693bb090b11a9f6f7443453 🚀
</commit_message>
<xml_diff>
--- a/2023/raw-fi.xlsx
+++ b/2023/raw-fi.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8327" uniqueCount="1468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8344" uniqueCount="1469">
   <si>
     <t>Timestamp</t>
   </si>
@@ -4417,6 +4417,9 @@
   </si>
   <si>
     <t>Fullstack web ja mobiili</t>
+  </si>
+  <si>
+    <t>Software architect, full-stack</t>
   </si>
 </sst>
 </file>
@@ -4690,7 +4693,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="32" width="18.88"/>
+    <col customWidth="1" min="1" max="19" width="18.88"/>
+    <col customWidth="1" min="20" max="20" width="51.38"/>
+    <col customWidth="1" min="21" max="32" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -49231,6 +49236,103 @@
       </c>
       <c r="N897" s="3" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" s="2">
+        <v>45193.938881458336</v>
+      </c>
+      <c r="B898" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C898" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D898" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F898" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H898" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="P898" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q898" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R898" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="S898" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="T898" s="3" t="s">
+        <v>1468</v>
+      </c>
+      <c r="U898" s="3">
+        <v>4500.0</v>
+      </c>
+      <c r="V898" s="3">
+        <v>60000.0</v>
+      </c>
+      <c r="X898" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" s="2">
+        <v>45193.98985868055</v>
+      </c>
+      <c r="B899" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C899" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D899" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E899" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F899" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="G899" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="H899" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="P899" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q899" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R899" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="S899" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="T899" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="U899" s="3">
+        <v>8500.0</v>
+      </c>
+      <c r="V899" s="3">
+        <v>102000.0</v>
+      </c>
+      <c r="W899" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="X899" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>